<commit_message>
update databricks lineage code
</commit_message>
<xml_diff>
--- a/scripts/Lineage inputs/51.15 Stackline Industry Visibility - Weekly Level - ACTIVEWEAR.xlsx
+++ b/scripts/Lineage inputs/51.15 Stackline Industry Visibility - Weekly Level - ACTIVEWEAR.xlsx
@@ -554,12 +554,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>common.dimstyle, StL.FACTATLASSALES, STL.DimRetailerSku, Explore.Amz_XrefUpc, StL.FactTrafficProducts, common.dimitem</t>
+          <t>STL.DimRetailerSku, common.dimstyle, common.dimitem, StL.FACTATLASSALES, Explore.Amz_XrefUpc, StL.FactTrafficProducts</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/common/dimstyle, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ StL/FACTATLASSALES, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ STL/DimRetailerSku, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ Explore/Amz_XrefUpc, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ StL/FactTrafficProducts, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ common/dimitem</t>
+          <t>mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/STL/DimRetailerSku, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ common/dimstyle, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ common/dimitem, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ StL/FACTATLASSALES, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ Explore/Amz_XrefUpc, mssql://hbi-pd01-analytics-dwsrv.database.windows.net/hbipd01dw/ StL/FactTrafficProducts</t>
         </is>
       </c>
     </row>

</xml_diff>